<commit_message>
Testes : Exercicios : Andamento
</commit_message>
<xml_diff>
--- a/testes/AS_exercicio.xlsx
+++ b/testes/AS_exercicio.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>Sistema:</t>
   </si>
@@ -119,28 +119,7 @@
     <t>Atualização</t>
   </si>
   <si>
-    <t>Associação existente no sistema</t>
-  </si>
-  <si>
     <t>CT008</t>
-  </si>
-  <si>
-    <t>Consultar associações</t>
-  </si>
-  <si>
-    <t>Exibição da tela de associação em modo de atualização</t>
-  </si>
-  <si>
-    <t>O Usuário Adm. Seleciona a opção de consultar associação</t>
-  </si>
-  <si>
-    <t>O sistema exibe uma nova tela com as associações existentes.</t>
-  </si>
-  <si>
-    <t>O sistem exibe a tela de associação em modo de atualização, com os dados do registro selecionado devidamente preenchidos.</t>
-  </si>
-  <si>
-    <t>Atualização de uma associação.</t>
   </si>
   <si>
     <t>CT008, CT009, o Usuario Adm. Realiza as alterações necessárias e clica no botão atualizar na parte inferior da tela</t>
@@ -164,9 +143,6 @@
     <t>Obrigatóriedade dos campos</t>
   </si>
   <si>
-    <t>Cliente dado obrigatório</t>
-  </si>
-  <si>
     <t xml:space="preserve">Inclusão: CT001, CT002       Atualização: CT008, CT009         </t>
   </si>
   <si>
@@ -176,28 +152,10 @@
     <t>Atualização: CT008, CT009</t>
   </si>
   <si>
-    <t>Exercício dado obrigatório</t>
-  </si>
-  <si>
     <t>Inclusão: CT001,CT002    Atualização: CT008, CT009</t>
   </si>
   <si>
-    <t>Equipamento dado obrigatório</t>
-  </si>
-  <si>
-    <t>Inclusão: CT001, CT002       Alteração: CT008, CT009</t>
-  </si>
-  <si>
-    <t>O Usuáriio Adm. Não selecionou um Cliente</t>
-  </si>
-  <si>
     <t>O sistema exibe uma mensagem no Toast informando que existem dados obrigatórios a serem preenchidos.</t>
-  </si>
-  <si>
-    <t>O Usuário Adm. Não selecionou um Exercício</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O Usuário Adm. Não selecionou um Equipamento </t>
   </si>
   <si>
     <t>RESULTADO DOS TESTES</t>
@@ -309,6 +267,42 @@
   </si>
   <si>
     <t>CT001, CT002, CT003</t>
+  </si>
+  <si>
+    <t>Consultar exercícios</t>
+  </si>
+  <si>
+    <t>No minímo um exercício cadastrado no sistema</t>
+  </si>
+  <si>
+    <t>O Usuário Adm. Seleciona a opção de consultar exercício.</t>
+  </si>
+  <si>
+    <t>O sistema exibe uma nova tela com os exercícios cadastrados.</t>
+  </si>
+  <si>
+    <t>Exibição da tela de cadastro de exercícios em modo de atualização</t>
+  </si>
+  <si>
+    <t>O sistema exibe a tela de cadastro de exercício em modo de atualização, com os dados do registro selecionado devidamente preenchidos.</t>
+  </si>
+  <si>
+    <t>Atualização de um exercício</t>
+  </si>
+  <si>
+    <t>Exercício cadastrado no sistema</t>
+  </si>
+  <si>
+    <t>nome do exercício  dado obrigatório</t>
+  </si>
+  <si>
+    <t>O Usuáriio Adm. Não preencheu o campo nome do exercício</t>
+  </si>
+  <si>
+    <t>Status do exercício dado obrigatório</t>
+  </si>
+  <si>
+    <t>O Usuário Adm. Não preencheu o campo status do  Exercício.</t>
   </si>
 </sst>
 </file>
@@ -431,7 +425,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,6 +489,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1158,7 +1164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1320,22 +1326,10 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1478,6 +1472,27 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="8" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2325,10 +2340,10 @@
   <dimension ref="A1:HV118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31:E33"/>
+      <selection pane="bottomRight" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2347,12 +2362,12 @@
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="112" t="s">
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="108" t="s">
         <v>19</v>
       </c>
       <c r="J1" s="1"/>
@@ -2581,12 +2596,12 @@
       <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="116" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="112" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="113"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="108"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -2810,13 +2825,13 @@
       <c r="HV2" s="1"/>
     </row>
     <row r="3" spans="1:230" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="119"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="112"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="108"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -3040,11 +3055,11 @@
       <c r="HV3" s="1"/>
     </row>
     <row r="4" spans="1:230" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="111"/>
-      <c r="B4" s="122"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="113"/>
+      <c r="A4" s="107"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="109"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -3268,13 +3283,13 @@
       <c r="HV4" s="1"/>
     </row>
     <row r="5" spans="1:230" s="4" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -3514,7 +3529,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -3739,22 +3754,22 @@
       <c r="HV6" s="1"/>
     </row>
     <row r="7" spans="1:230" s="8" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="97" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="97" t="s">
+      <c r="B7" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="93" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="81"/>
+        <v>47</v>
+      </c>
+      <c r="F7" s="77"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
@@ -3978,12 +3993,12 @@
       <c r="HV7" s="12"/>
     </row>
     <row r="8" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="92"/>
       <c r="D8" s="46"/>
       <c r="E8" s="48"/>
-      <c r="F8" s="82"/>
+      <c r="F8" s="78"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
@@ -4207,12 +4222,12 @@
       <c r="HV8" s="12"/>
     </row>
     <row r="9" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="96"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
       <c r="D9" s="46"/>
       <c r="E9" s="48"/>
-      <c r="F9" s="82"/>
+      <c r="F9" s="78"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -4665,22 +4680,22 @@
       <c r="HV10"/>
     </row>
     <row r="11" spans="1:230" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="127">
+      <c r="A11" s="123">
         <v>2</v>
       </c>
-      <c r="B11" s="103" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="103" t="s">
+      <c r="B11" s="99" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="99" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E11" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="83"/>
+        <v>51</v>
+      </c>
+      <c r="F11" s="79"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -4904,14 +4919,14 @@
       <c r="HV11" s="12"/>
     </row>
     <row r="12" spans="1:230" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="90"/>
-      <c r="B12" s="104"/>
-      <c r="C12" s="104"/>
+      <c r="A12" s="86"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="46" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E12" s="47"/>
-      <c r="F12" s="83"/>
+      <c r="F12" s="79"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
@@ -5135,14 +5150,14 @@
       <c r="HV12" s="12"/>
     </row>
     <row r="13" spans="1:230" s="8" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="91"/>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
+      <c r="A13" s="87"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="101"/>
       <c r="D13" s="46" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="47"/>
-      <c r="F13" s="83"/>
+      <c r="F13" s="79"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
@@ -5595,22 +5610,22 @@
       <c r="HV14"/>
     </row>
     <row r="15" spans="1:230" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="127" t="s">
+      <c r="A15" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="103" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="103" t="s">
-        <v>67</v>
+      <c r="B15" s="99" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="99" t="s">
+        <v>53</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="81"/>
+        <v>55</v>
+      </c>
+      <c r="F15" s="77"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
@@ -5834,12 +5849,12 @@
       <c r="HV15" s="12"/>
     </row>
     <row r="16" spans="1:230" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="90"/>
-      <c r="B16" s="104"/>
-      <c r="C16" s="104"/>
+      <c r="A16" s="86"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
       <c r="D16" s="46"/>
       <c r="E16" s="48"/>
-      <c r="F16" s="81"/>
+      <c r="F16" s="77"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
@@ -6063,12 +6078,12 @@
       <c r="HV16" s="12"/>
     </row>
     <row r="17" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="91"/>
-      <c r="B17" s="105"/>
-      <c r="C17" s="105"/>
+      <c r="A17" s="87"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="101"/>
       <c r="D17" s="46"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="81"/>
+      <c r="F17" s="77"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
@@ -6521,22 +6536,22 @@
       <c r="HV18"/>
     </row>
     <row r="19" spans="1:230" s="8" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="97" t="s">
+      <c r="B19" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="97" t="s">
-        <v>70</v>
+      <c r="C19" s="93" t="s">
+        <v>56</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E19" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="84"/>
+      <c r="F19" s="80"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -6760,12 +6775,12 @@
       <c r="HV19" s="12"/>
     </row>
     <row r="20" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="78"/>
-      <c r="B20" s="96"/>
-      <c r="C20" s="96"/>
+      <c r="A20" s="74"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="92"/>
       <c r="D20" s="46"/>
       <c r="E20" s="48"/>
-      <c r="F20" s="82"/>
+      <c r="F20" s="78"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
@@ -6989,12 +7004,12 @@
       <c r="HV20" s="12"/>
     </row>
     <row r="21" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="78"/>
-      <c r="B21" s="96"/>
-      <c r="C21" s="96"/>
+      <c r="A21" s="74"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
       <c r="D21" s="46"/>
       <c r="E21" s="48"/>
-      <c r="F21" s="82"/>
+      <c r="F21" s="78"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
@@ -7447,30 +7462,30 @@
       <c r="HV22"/>
     </row>
     <row r="23" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="77">
+      <c r="A23" s="73">
         <v>5</v>
       </c>
-      <c r="B23" s="97"/>
-      <c r="C23" s="97"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="93"/>
       <c r="D23" s="46"/>
       <c r="E23" s="48"/>
-      <c r="F23" s="85"/>
+      <c r="F23" s="81"/>
     </row>
     <row r="24" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="78"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="96"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="46"/>
       <c r="E24" s="48"/>
-      <c r="F24" s="73"/>
+      <c r="F24" s="71"/>
     </row>
     <row r="25" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="78"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
+      <c r="A25" s="74"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="92"/>
       <c r="D25" s="46"/>
       <c r="E25" s="48"/>
-      <c r="F25" s="73"/>
+      <c r="F25" s="71"/>
     </row>
     <row r="26" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
@@ -7481,30 +7496,30 @@
       <c r="F26" s="51"/>
     </row>
     <row r="27" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="77">
+      <c r="A27" s="73">
         <v>6</v>
       </c>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="93"/>
       <c r="D27" s="46"/>
       <c r="E27" s="48"/>
-      <c r="F27" s="85"/>
+      <c r="F27" s="81"/>
     </row>
     <row r="28" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="78"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="92"/>
+      <c r="C28" s="92"/>
       <c r="D28" s="46"/>
       <c r="E28" s="48"/>
-      <c r="F28" s="75"/>
+      <c r="F28" s="72"/>
     </row>
     <row r="29" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="78"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="96"/>
+      <c r="A29" s="74"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="92"/>
       <c r="D29" s="46"/>
       <c r="E29" s="48"/>
-      <c r="F29" s="75"/>
+      <c r="F29" s="72"/>
     </row>
     <row r="30" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
@@ -7514,81 +7529,81 @@
       <c r="E30" s="50"/>
     </row>
     <row r="31" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="77">
+      <c r="A31" s="73">
         <v>7</v>
       </c>
-      <c r="B31" s="97"/>
-      <c r="C31" s="97"/>
+      <c r="B31" s="93"/>
+      <c r="C31" s="93"/>
       <c r="D31" s="46"/>
       <c r="E31" s="48"/>
-      <c r="F31" s="85"/>
+      <c r="F31" s="81"/>
     </row>
     <row r="32" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="107"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="96"/>
+      <c r="A32" s="103"/>
+      <c r="B32" s="92"/>
+      <c r="C32" s="92"/>
       <c r="D32" s="46"/>
       <c r="E32" s="48"/>
-      <c r="F32" s="75"/>
+      <c r="F32" s="72"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
+      <c r="A33" s="103"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="92"/>
       <c r="D33" s="46"/>
       <c r="E33" s="48"/>
-      <c r="F33" s="75"/>
+      <c r="F33" s="72"/>
     </row>
     <row r="34" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="108" t="s">
+      <c r="A34" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="109"/>
-      <c r="C34" s="109"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="109"/>
+      <c r="B34" s="105"/>
+      <c r="C34" s="105"/>
+      <c r="D34" s="105"/>
+      <c r="E34" s="105"/>
     </row>
     <row r="35" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="77">
+      <c r="A35" s="73">
         <v>8</v>
       </c>
-      <c r="B35" s="97" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="97" t="s">
-        <v>29</v>
+      <c r="B35" s="93" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="93" t="s">
+        <v>58</v>
       </c>
       <c r="D35" s="46" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="E35" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="74"/>
+        <v>60</v>
+      </c>
+      <c r="F35" s="124"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="78"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="96"/>
+      <c r="A36" s="74"/>
+      <c r="B36" s="92"/>
+      <c r="C36" s="92"/>
       <c r="D36" s="46"/>
       <c r="E36" s="48"/>
-      <c r="F36" s="75"/>
+      <c r="F36" s="125"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="78"/>
-      <c r="B37" s="96"/>
-      <c r="C37" s="96"/>
+      <c r="A37" s="74"/>
+      <c r="B37" s="92"/>
+      <c r="C37" s="92"/>
       <c r="D37" s="46"/>
       <c r="E37" s="48"/>
-      <c r="F37" s="75"/>
+      <c r="F37" s="125"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="78"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="96"/>
+      <c r="A38" s="74"/>
+      <c r="B38" s="92"/>
+      <c r="C38" s="92"/>
       <c r="D38" s="46"/>
       <c r="E38" s="48"/>
-      <c r="F38" s="75"/>
+      <c r="F38" s="125"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="37"/>
@@ -7598,40 +7613,40 @@
       <c r="E39" s="50"/>
     </row>
     <row r="40" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="77">
+      <c r="A40" s="73">
         <v>9</v>
       </c>
-      <c r="B40" s="97" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="106" t="s">
-        <v>30</v>
+      <c r="B40" s="93" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="102" t="s">
+        <v>29</v>
       </c>
       <c r="D40" s="46" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E40" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" s="74"/>
+        <v>62</v>
+      </c>
+      <c r="F40" s="124"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="78"/>
-      <c r="B41" s="96"/>
-      <c r="C41" s="104"/>
+      <c r="A41" s="74"/>
+      <c r="B41" s="92"/>
+      <c r="C41" s="100"/>
       <c r="D41" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E41" s="48"/>
-      <c r="F41" s="75"/>
+      <c r="F41" s="125"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="78"/>
-      <c r="B42" s="96"/>
-      <c r="C42" s="95"/>
+      <c r="A42" s="74"/>
+      <c r="B42" s="92"/>
+      <c r="C42" s="91"/>
       <c r="D42" s="46"/>
       <c r="E42" s="48"/>
-      <c r="F42" s="75"/>
+      <c r="F42" s="125"/>
     </row>
     <row r="43" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="37"/>
@@ -7641,38 +7656,38 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="77">
+      <c r="A44" s="73">
         <v>10</v>
       </c>
-      <c r="B44" s="103" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="106" t="s">
-        <v>29</v>
+      <c r="B44" s="99" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="102" t="s">
+        <v>64</v>
       </c>
       <c r="D44" s="46" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E44" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="73"/>
+        <v>31</v>
+      </c>
+      <c r="F44" s="126"/>
     </row>
     <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="78"/>
-      <c r="B45" s="104"/>
-      <c r="C45" s="104"/>
+      <c r="A45" s="74"/>
+      <c r="B45" s="100"/>
+      <c r="C45" s="100"/>
       <c r="D45" s="46"/>
       <c r="E45" s="48"/>
-      <c r="F45" s="73"/>
+      <c r="F45" s="126"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="78"/>
-      <c r="B46" s="105"/>
-      <c r="C46" s="105"/>
+      <c r="A46" s="74"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="101"/>
       <c r="D46" s="52"/>
       <c r="E46" s="48"/>
-      <c r="F46" s="73"/>
+      <c r="F46" s="126"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="37"/>
@@ -7683,38 +7698,38 @@
       <c r="F47" s="51"/>
     </row>
     <row r="48" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="77">
+      <c r="A48" s="73">
         <v>11</v>
       </c>
-      <c r="B48" s="98" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" s="98" t="s">
-        <v>40</v>
+      <c r="B48" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="94" t="s">
+        <v>33</v>
       </c>
       <c r="D48" s="46" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E48" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" s="73"/>
+        <v>34</v>
+      </c>
+      <c r="F48" s="126"/>
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="78"/>
-      <c r="B49" s="99"/>
-      <c r="C49" s="99"/>
+      <c r="A49" s="74"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
       <c r="D49" s="46"/>
       <c r="E49" s="48"/>
-      <c r="F49" s="73"/>
+      <c r="F49" s="126"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="78"/>
-      <c r="B50" s="100"/>
-      <c r="C50" s="100"/>
+      <c r="A50" s="74"/>
+      <c r="B50" s="96"/>
+      <c r="C50" s="96"/>
       <c r="D50" s="52"/>
       <c r="E50" s="53"/>
-      <c r="F50" s="73"/>
+      <c r="F50" s="126"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="37"/>
@@ -7725,88 +7740,88 @@
       <c r="F51" s="51"/>
     </row>
     <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="77">
+      <c r="A52" s="73">
         <v>12</v>
       </c>
-      <c r="B52" s="101" t="s">
+      <c r="B52" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="102" t="s">
-        <v>42</v>
+      <c r="C52" s="98" t="s">
+        <v>35</v>
       </c>
       <c r="D52" s="55" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E52" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="F52" s="76"/>
+      <c r="F52" s="127"/>
     </row>
     <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="78"/>
-      <c r="B53" s="101"/>
-      <c r="C53" s="102"/>
+      <c r="A53" s="74"/>
+      <c r="B53" s="97"/>
+      <c r="C53" s="98"/>
       <c r="D53" s="57"/>
       <c r="E53" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F53" s="76"/>
+      <c r="F53" s="127"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="78"/>
-      <c r="B54" s="101"/>
-      <c r="C54" s="102"/>
+      <c r="A54" s="74"/>
+      <c r="B54" s="97"/>
+      <c r="C54" s="98"/>
       <c r="D54" s="58"/>
       <c r="E54" s="59"/>
-      <c r="F54" s="76"/>
+      <c r="F54" s="127"/>
     </row>
     <row r="55" spans="1:6" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="87" t="s">
-        <v>43</v>
-      </c>
-      <c r="B55" s="88"/>
-      <c r="C55" s="88"/>
-      <c r="D55" s="88"/>
-      <c r="E55" s="88"/>
+      <c r="A55" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="84"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="84"/>
       <c r="F55" s="51"/>
     </row>
     <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A56" s="77">
+      <c r="A56" s="73">
         <v>13</v>
       </c>
-      <c r="B56" s="101" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" s="102" t="s">
-        <v>45</v>
+      <c r="B56" s="97" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="98" t="s">
+        <v>37</v>
       </c>
       <c r="D56" s="55" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E56" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="F56" s="71"/>
+        <v>41</v>
+      </c>
+      <c r="F56" s="128"/>
     </row>
     <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="78"/>
-      <c r="B57" s="101"/>
-      <c r="C57" s="102"/>
+      <c r="A57" s="74"/>
+      <c r="B57" s="97"/>
+      <c r="C57" s="98"/>
       <c r="D57" s="61" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E57" s="62"/>
-      <c r="F57" s="71"/>
+      <c r="F57" s="128"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="78"/>
-      <c r="B58" s="101"/>
-      <c r="C58" s="102"/>
+      <c r="A58" s="74"/>
+      <c r="B58" s="97"/>
+      <c r="C58" s="98"/>
       <c r="D58" s="63" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E58" s="64"/>
-      <c r="F58" s="71"/>
+      <c r="F58" s="128"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="37"/>
@@ -7817,42 +7832,42 @@
       <c r="F59" s="51"/>
     </row>
     <row r="60" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="77">
+      <c r="A60" s="73">
         <v>14</v>
       </c>
-      <c r="B60" s="101" t="s">
-        <v>48</v>
-      </c>
-      <c r="C60" s="102" t="s">
-        <v>49</v>
+      <c r="B60" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" s="98" t="s">
+        <v>40</v>
       </c>
       <c r="D60" s="66" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E60" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="F60" s="72"/>
+        <v>41</v>
+      </c>
+      <c r="F60" s="129"/>
     </row>
     <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="78"/>
-      <c r="B61" s="101"/>
-      <c r="C61" s="101"/>
+      <c r="A61" s="74"/>
+      <c r="B61" s="97"/>
+      <c r="C61" s="97"/>
       <c r="D61" s="67" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E61" s="67"/>
-      <c r="F61" s="72"/>
+      <c r="F61" s="129"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="78"/>
-      <c r="B62" s="101"/>
-      <c r="C62" s="101"/>
+      <c r="A62" s="74"/>
+      <c r="B62" s="97"/>
+      <c r="C62" s="97"/>
       <c r="D62" s="67" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E62" s="67"/>
-      <c r="F62" s="72"/>
+      <c r="F62" s="129"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37"/>
@@ -7862,43 +7877,31 @@
       <c r="E63" s="50"/>
       <c r="F63" s="51"/>
     </row>
-    <row r="64" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="77">
+    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="73">
         <v>15</v>
       </c>
-      <c r="B64" s="95" t="s">
-        <v>50</v>
-      </c>
-      <c r="C64" s="95" t="s">
-        <v>51</v>
-      </c>
-      <c r="D64" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="E64" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="F64" s="73"/>
+      <c r="B64" s="91"/>
+      <c r="C64" s="91"/>
+      <c r="D64" s="46"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="130"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="78"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="96"/>
-      <c r="D65" s="46" t="s">
-        <v>47</v>
-      </c>
+      <c r="A65" s="74"/>
+      <c r="B65" s="92"/>
+      <c r="C65" s="92"/>
+      <c r="D65" s="46"/>
       <c r="E65" s="48"/>
-      <c r="F65" s="73"/>
+      <c r="F65" s="130"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="78"/>
-      <c r="B66" s="96"/>
-      <c r="C66" s="96"/>
-      <c r="D66" s="46" t="s">
-        <v>55</v>
-      </c>
+      <c r="A66" s="74"/>
+      <c r="B66" s="92"/>
+      <c r="C66" s="92"/>
+      <c r="D66" s="46"/>
       <c r="E66" s="48"/>
-      <c r="F66" s="73"/>
+      <c r="F66" s="130"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37"/>
@@ -7909,11 +7912,11 @@
       <c r="F67" s="51"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="77">
+      <c r="A68" s="73">
         <v>16</v>
       </c>
-      <c r="B68" s="97"/>
-      <c r="C68" s="97" t="s">
+      <c r="B68" s="93"/>
+      <c r="C68" s="93" t="s">
         <v>17</v>
       </c>
       <c r="D68" s="46"/>
@@ -7921,17 +7924,17 @@
       <c r="F68" s="51"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="78"/>
-      <c r="B69" s="96"/>
-      <c r="C69" s="96"/>
+      <c r="A69" s="74"/>
+      <c r="B69" s="92"/>
+      <c r="C69" s="92"/>
       <c r="D69" s="46"/>
       <c r="E69" s="48"/>
       <c r="F69" s="51"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="78"/>
-      <c r="B70" s="96"/>
-      <c r="C70" s="96"/>
+      <c r="A70" s="74"/>
+      <c r="B70" s="92"/>
+      <c r="C70" s="92"/>
       <c r="D70" s="46"/>
       <c r="E70" s="48"/>
       <c r="F70" s="51"/>
@@ -7946,25 +7949,25 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="77">
+      <c r="A72" s="73">
         <v>17</v>
       </c>
-      <c r="B72" s="79"/>
-      <c r="C72" s="79"/>
+      <c r="B72" s="75"/>
+      <c r="C72" s="75"/>
       <c r="D72" s="40"/>
       <c r="E72" s="41"/>
     </row>
     <row r="73" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="78"/>
-      <c r="B73" s="86"/>
-      <c r="C73" s="86"/>
+      <c r="A73" s="74"/>
+      <c r="B73" s="82"/>
+      <c r="C73" s="82"/>
       <c r="D73" s="40"/>
       <c r="E73" s="41"/>
     </row>
     <row r="74" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="78"/>
-      <c r="B74" s="86"/>
-      <c r="C74" s="86"/>
+      <c r="A74" s="74"/>
+      <c r="B74" s="82"/>
+      <c r="C74" s="82"/>
       <c r="D74" s="42" t="s">
         <v>16</v>
       </c>
@@ -7980,25 +7983,25 @@
       <c r="E75" s="39"/>
     </row>
     <row r="76" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="77">
+      <c r="A76" s="73">
         <v>18</v>
       </c>
-      <c r="B76" s="79"/>
-      <c r="C76" s="79"/>
+      <c r="B76" s="75"/>
+      <c r="C76" s="75"/>
       <c r="D76" s="40"/>
       <c r="E76" s="41"/>
     </row>
     <row r="77" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="78"/>
-      <c r="B77" s="86"/>
-      <c r="C77" s="86"/>
+      <c r="A77" s="74"/>
+      <c r="B77" s="82"/>
+      <c r="C77" s="82"/>
       <c r="D77" s="40"/>
       <c r="E77" s="41"/>
     </row>
     <row r="78" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="78"/>
-      <c r="B78" s="86"/>
-      <c r="C78" s="86"/>
+      <c r="A78" s="74"/>
+      <c r="B78" s="82"/>
+      <c r="C78" s="82"/>
       <c r="D78" s="42" t="s">
         <v>16</v>
       </c>
@@ -8014,23 +8017,23 @@
       <c r="E79" s="39"/>
     </row>
     <row r="80" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="77"/>
-      <c r="B80" s="79"/>
-      <c r="C80" s="79"/>
+      <c r="A80" s="73"/>
+      <c r="B80" s="75"/>
+      <c r="C80" s="75"/>
       <c r="D80" s="40"/>
       <c r="E80" s="41"/>
     </row>
     <row r="81" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="78"/>
-      <c r="B81" s="80"/>
-      <c r="C81" s="80"/>
+      <c r="A81" s="74"/>
+      <c r="B81" s="76"/>
+      <c r="C81" s="76"/>
       <c r="D81" s="40"/>
       <c r="E81" s="41"/>
     </row>
     <row r="82" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="78"/>
-      <c r="B82" s="80"/>
-      <c r="C82" s="80"/>
+      <c r="A82" s="74"/>
+      <c r="B82" s="76"/>
+      <c r="C82" s="76"/>
       <c r="D82" s="40"/>
       <c r="E82" s="41"/>
     </row>
@@ -8042,23 +8045,23 @@
       <c r="E83" s="44"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="77"/>
-      <c r="B84" s="79"/>
-      <c r="C84" s="79"/>
+      <c r="A84" s="73"/>
+      <c r="B84" s="75"/>
+      <c r="C84" s="75"/>
       <c r="D84" s="40"/>
       <c r="E84" s="41"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="78"/>
-      <c r="B85" s="80"/>
-      <c r="C85" s="80"/>
+      <c r="A85" s="74"/>
+      <c r="B85" s="76"/>
+      <c r="C85" s="76"/>
       <c r="D85" s="40"/>
       <c r="E85" s="41"/>
     </row>
     <row r="86" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="78"/>
-      <c r="B86" s="80"/>
-      <c r="C86" s="80"/>
+      <c r="A86" s="74"/>
+      <c r="B86" s="76"/>
+      <c r="C86" s="76"/>
       <c r="D86" s="40"/>
       <c r="E86" s="41"/>
     </row>
@@ -8070,23 +8073,23 @@
       <c r="E87" s="44"/>
     </row>
     <row r="88" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="77"/>
-      <c r="B88" s="79"/>
-      <c r="C88" s="79"/>
+      <c r="A88" s="73"/>
+      <c r="B88" s="75"/>
+      <c r="C88" s="75"/>
       <c r="D88" s="40"/>
       <c r="E88" s="41"/>
     </row>
     <row r="89" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="78"/>
-      <c r="B89" s="80"/>
-      <c r="C89" s="80"/>
+      <c r="A89" s="74"/>
+      <c r="B89" s="76"/>
+      <c r="C89" s="76"/>
       <c r="D89" s="40"/>
       <c r="E89" s="41"/>
     </row>
     <row r="90" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="78"/>
-      <c r="B90" s="80"/>
-      <c r="C90" s="80"/>
+      <c r="A90" s="74"/>
+      <c r="B90" s="76"/>
+      <c r="C90" s="76"/>
       <c r="D90" s="40"/>
       <c r="E90" s="41"/>
     </row>
@@ -8098,23 +8101,23 @@
       <c r="E91" s="44"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="77"/>
-      <c r="B92" s="79"/>
-      <c r="C92" s="79"/>
+      <c r="A92" s="73"/>
+      <c r="B92" s="75"/>
+      <c r="C92" s="75"/>
       <c r="D92" s="40"/>
       <c r="E92" s="41"/>
     </row>
     <row r="93" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="78"/>
-      <c r="B93" s="80"/>
-      <c r="C93" s="80"/>
+      <c r="A93" s="74"/>
+      <c r="B93" s="76"/>
+      <c r="C93" s="76"/>
       <c r="D93" s="40"/>
       <c r="E93" s="41"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="78"/>
-      <c r="B94" s="80"/>
-      <c r="C94" s="80"/>
+      <c r="A94" s="74"/>
+      <c r="B94" s="76"/>
+      <c r="C94" s="76"/>
       <c r="D94" s="40"/>
       <c r="E94" s="41"/>
     </row>
@@ -8126,23 +8129,23 @@
       <c r="E95" s="44"/>
     </row>
     <row r="96" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="77"/>
-      <c r="B96" s="79"/>
-      <c r="C96" s="79"/>
+      <c r="A96" s="73"/>
+      <c r="B96" s="75"/>
+      <c r="C96" s="75"/>
       <c r="D96" s="40"/>
       <c r="E96" s="41"/>
     </row>
     <row r="97" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="78"/>
-      <c r="B97" s="80"/>
-      <c r="C97" s="80"/>
+      <c r="A97" s="74"/>
+      <c r="B97" s="76"/>
+      <c r="C97" s="76"/>
       <c r="D97" s="40"/>
       <c r="E97" s="41"/>
     </row>
     <row r="98" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="78"/>
-      <c r="B98" s="80"/>
-      <c r="C98" s="80"/>
+      <c r="A98" s="74"/>
+      <c r="B98" s="76"/>
+      <c r="C98" s="76"/>
       <c r="D98" s="40"/>
       <c r="E98" s="41"/>
     </row>
@@ -8154,23 +8157,23 @@
       <c r="E99" s="44"/>
     </row>
     <row r="100" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="77"/>
-      <c r="B100" s="79"/>
-      <c r="C100" s="79"/>
+      <c r="A100" s="73"/>
+      <c r="B100" s="75"/>
+      <c r="C100" s="75"/>
       <c r="D100" s="40"/>
       <c r="E100" s="41"/>
     </row>
     <row r="101" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="78"/>
-      <c r="B101" s="80"/>
-      <c r="C101" s="80"/>
+      <c r="A101" s="74"/>
+      <c r="B101" s="76"/>
+      <c r="C101" s="76"/>
       <c r="D101" s="40"/>
       <c r="E101" s="41"/>
     </row>
     <row r="102" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="78"/>
-      <c r="B102" s="80"/>
-      <c r="C102" s="80"/>
+      <c r="A102" s="74"/>
+      <c r="B102" s="76"/>
+      <c r="C102" s="76"/>
       <c r="D102" s="40"/>
       <c r="E102" s="41"/>
     </row>
@@ -8182,23 +8185,23 @@
       <c r="E103" s="44"/>
     </row>
     <row r="104" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="77"/>
-      <c r="B104" s="79"/>
-      <c r="C104" s="79"/>
+      <c r="A104" s="73"/>
+      <c r="B104" s="75"/>
+      <c r="C104" s="75"/>
       <c r="D104" s="40"/>
       <c r="E104" s="41"/>
     </row>
     <row r="105" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="78"/>
-      <c r="B105" s="80"/>
-      <c r="C105" s="80"/>
+      <c r="A105" s="74"/>
+      <c r="B105" s="76"/>
+      <c r="C105" s="76"/>
       <c r="D105" s="40"/>
       <c r="E105" s="41"/>
     </row>
     <row r="106" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="78"/>
-      <c r="B106" s="80"/>
-      <c r="C106" s="80"/>
+      <c r="A106" s="74"/>
+      <c r="B106" s="76"/>
+      <c r="C106" s="76"/>
       <c r="D106" s="40"/>
       <c r="E106" s="41"/>
     </row>
@@ -8210,23 +8213,23 @@
       <c r="E107" s="44"/>
     </row>
     <row r="108" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="77"/>
-      <c r="B108" s="79"/>
-      <c r="C108" s="79"/>
+      <c r="A108" s="73"/>
+      <c r="B108" s="75"/>
+      <c r="C108" s="75"/>
       <c r="D108" s="40"/>
       <c r="E108" s="41"/>
     </row>
     <row r="109" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="78"/>
-      <c r="B109" s="80"/>
-      <c r="C109" s="80"/>
+      <c r="A109" s="74"/>
+      <c r="B109" s="76"/>
+      <c r="C109" s="76"/>
       <c r="D109" s="40"/>
       <c r="E109" s="41"/>
     </row>
     <row r="110" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="78"/>
-      <c r="B110" s="80"/>
-      <c r="C110" s="80"/>
+      <c r="A110" s="74"/>
+      <c r="B110" s="76"/>
+      <c r="C110" s="76"/>
       <c r="D110" s="40"/>
       <c r="E110" s="41"/>
     </row>
@@ -8238,23 +8241,23 @@
       <c r="E111" s="44"/>
     </row>
     <row r="112" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="77"/>
-      <c r="B112" s="79"/>
-      <c r="C112" s="79"/>
+      <c r="A112" s="73"/>
+      <c r="B112" s="75"/>
+      <c r="C112" s="75"/>
       <c r="D112" s="40"/>
       <c r="E112" s="41"/>
     </row>
     <row r="113" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="78"/>
-      <c r="B113" s="80"/>
-      <c r="C113" s="80"/>
+      <c r="A113" s="74"/>
+      <c r="B113" s="76"/>
+      <c r="C113" s="76"/>
       <c r="D113" s="40"/>
       <c r="E113" s="41"/>
     </row>
     <row r="114" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="78"/>
-      <c r="B114" s="80"/>
-      <c r="C114" s="80"/>
+      <c r="A114" s="74"/>
+      <c r="B114" s="76"/>
+      <c r="C114" s="76"/>
       <c r="D114" s="40"/>
       <c r="E114" s="41"/>
     </row>
@@ -8266,23 +8269,23 @@
       <c r="E115" s="44"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="89"/>
-      <c r="B116" s="92"/>
-      <c r="C116" s="92"/>
+      <c r="A116" s="85"/>
+      <c r="B116" s="88"/>
+      <c r="C116" s="88"/>
       <c r="D116" s="40"/>
       <c r="E116" s="41"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="90"/>
-      <c r="B117" s="93"/>
-      <c r="C117" s="93"/>
+      <c r="A117" s="86"/>
+      <c r="B117" s="89"/>
+      <c r="C117" s="89"/>
       <c r="D117" s="40"/>
       <c r="E117" s="41"/>
     </row>
     <row r="118" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="91"/>
-      <c r="B118" s="94"/>
-      <c r="C118" s="94"/>
+      <c r="A118" s="87"/>
+      <c r="B118" s="90"/>
+      <c r="C118" s="90"/>
       <c r="D118" s="40"/>
       <c r="E118" s="41"/>
     </row>

</xml_diff>